<commit_message>
Funções com Pandas e criação de dataframe
</commit_message>
<xml_diff>
--- a/workplace.xlsx
+++ b/workplace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ulyss\OneDrive\Área de Trabalho\Curso Pós Graduação em Analise de Dados\PythonEstatistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA23904-EA52-4A7B-90D3-E9B946989689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9DF87F-CFFD-49E1-A6EE-9004B6EBB381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{748FDA57-4FAD-41BF-88CE-4EC82A7CFF50}"/>
+    <workbookView xWindow="10200" yWindow="0" windowWidth="10200" windowHeight="10920" xr2:uid="{748FDA57-4FAD-41BF-88CE-4EC82A7CFF50}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE694223-3285-43A9-AE5A-0B82D944C66A}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:E24"/>
@@ -535,7 +535,7 @@
         <v>1.2</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E23" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E24" si="0">C3*D3</f>
         <v>27.599999999999998</v>
       </c>
     </row>
@@ -898,6 +898,10 @@
         <f t="shared" si="0"/>
         <v>26.4</v>
       </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+      <c r="E24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>